<commit_message>
Added rsi, macd and atr in cron
</commit_message>
<xml_diff>
--- a/assets/Book1.xlsx
+++ b/assets/Book1.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\algo-trade\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32BF1F98-A1F7-490C-A5C9-9179A02AD194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01EAEBA2-9344-412D-8175-360CC1035C47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4A377C6A-B5AE-41A3-93E6-B24FE0D52FEA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{4A377C6A-B5AE-41A3-93E6-B24FE0D52FEA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$26</definedName>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="33">
   <si>
     <t>Strong Sell</t>
   </si>
@@ -98,6 +99,45 @@
   </si>
   <si>
     <t>1minTrend</t>
+  </si>
+  <si>
+    <t>momentum_rsi</t>
+  </si>
+  <si>
+    <t>trend_macd</t>
+  </si>
+  <si>
+    <t>volatility_atr</t>
+  </si>
+  <si>
+    <t>buy</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>sell</t>
+  </si>
+  <si>
+    <t>no_order</t>
+  </si>
+  <si>
+    <t>buy_order</t>
+  </si>
+  <si>
+    <t>sell_order</t>
+  </si>
+  <si>
+    <t>hold</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>exit</t>
   </si>
 </sst>
 </file>
@@ -489,7 +529,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58F87E7E-8EDA-4AA3-AD7B-4DF0A29D178D}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -1010,4 +1050,405 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB0B43F8-2FDA-4765-AC0F-F76127D715E4}">
+  <dimension ref="A1:F19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.5546875" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>